<commit_message>
Pequenos aprimoramentos no site antigo
</commit_message>
<xml_diff>
--- a/Sprint2/Documentação/TI/Backlogs/Backlog_S2.xlsx
+++ b/Sprint2/Documentação/TI/Backlogs/Backlog_S2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\desen\OneDrive - SPTech School\Sptech\Pesquisa e Inovação\Grupo 06\Backlog - S2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\desen\Documents\programação\repositorioPi_Grupo06\Sprint2\Documentação\TI\Backlogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8681E098-EF9C-4E3D-864C-3C0EE08131E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FD06BF-25AF-48CD-8FC2-231D05D43325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{38A01445-BA88-473F-90C8-EC5411C7FC48}"/>
   </bookViews>
@@ -235,9 +235,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -245,6 +242,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -585,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A2BE7FB-8AA6-4E1B-9FDB-3DDEBA1790AD}">
   <dimension ref="F6:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" zoomScale="92" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,12 +600,12 @@
   </cols>
   <sheetData>
     <row r="6" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
     </row>
     <row r="7" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F7" s="1" t="s">
@@ -628,10 +628,10 @@
       <c r="G8" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" s="5" t="s">
+      <c r="H8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>37</v>
       </c>
     </row>
@@ -642,10 +642,10 @@
       <c r="G9" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I9" s="5" t="s">
+      <c r="H9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>37</v>
       </c>
     </row>
@@ -656,11 +656,11 @@
       <c r="G10" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>37</v>
+      <c r="H10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="6:9" x14ac:dyDescent="0.25">
@@ -670,10 +670,10 @@
       <c r="G11" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I11" s="4" t="s">
+      <c r="H11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -684,11 +684,11 @@
       <c r="G12" t="s">
         <v>24</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>37</v>
+      <c r="H12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="6:9" x14ac:dyDescent="0.25">
@@ -698,10 +698,10 @@
       <c r="G13" t="s">
         <v>25</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13" s="5" t="s">
+      <c r="H13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="4" t="s">
         <v>37</v>
       </c>
     </row>
@@ -712,10 +712,10 @@
       <c r="G14" t="s">
         <v>26</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" s="5" t="s">
+      <c r="H14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" s="4" t="s">
         <v>37</v>
       </c>
     </row>
@@ -726,10 +726,10 @@
       <c r="G15" t="s">
         <v>27</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I15" s="5" t="s">
+      <c r="H15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="4" t="s">
         <v>37</v>
       </c>
     </row>
@@ -740,11 +740,11 @@
       <c r="G16" t="s">
         <v>28</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="2" t="s">
         <v>35</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="6:9" x14ac:dyDescent="0.25">
@@ -754,10 +754,10 @@
       <c r="G17" t="s">
         <v>29</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I17" s="5" t="s">
+      <c r="H17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" s="4" t="s">
         <v>37</v>
       </c>
     </row>
@@ -768,11 +768,11 @@
       <c r="G18" t="s">
         <v>30</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>37</v>
+      <c r="H18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="6:9" x14ac:dyDescent="0.25">
@@ -782,11 +782,11 @@
       <c r="G19" t="s">
         <v>31</v>
       </c>
-      <c r="H19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>37</v>
+      <c r="H19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="6:9" x14ac:dyDescent="0.25">
@@ -796,11 +796,11 @@
       <c r="G20" t="s">
         <v>32</v>
       </c>
-      <c r="H20" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>37</v>
+      <c r="H20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="6:9" x14ac:dyDescent="0.25">
@@ -810,11 +810,11 @@
       <c r="G21" t="s">
         <v>33</v>
       </c>
-      <c r="H21" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>37</v>
+      <c r="H21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="6:9" x14ac:dyDescent="0.25">
@@ -824,10 +824,10 @@
       <c r="G22" t="s">
         <v>34</v>
       </c>
-      <c r="H22" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I22" s="5" t="s">
+      <c r="H22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I22" s="4" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>